<commit_message>
starting with email formatting
</commit_message>
<xml_diff>
--- a/testes-automation.xlsx
+++ b/testes-automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo LP\Documents\Python\Projeto automação - TESTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9D88D-69D1-4A12-B96B-55CDFCCC6CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF04592-C36A-4D68-AE69-4317FC24B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8FB530B9-8276-4415-81AE-BC5B4A3A5C09}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>123</v>
+        <v>40412</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>223</v>
+        <v>40416</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
ajustes em formatação de emails e ajustes para testes
</commit_message>
<xml_diff>
--- a/testes-automation.xlsx
+++ b/testes-automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo LP\Documents\Python\Projeto automação - TESTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF04592-C36A-4D68-AE69-4317FC24B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6067DEA-DBC0-40A8-A34C-0D1BA6754918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8FB530B9-8276-4415-81AE-BC5B4A3A5C09}"/>
   </bookViews>
@@ -71,13 +71,13 @@
     <t>ajustar ccomandos</t>
   </si>
   <si>
-    <t>MEB melhoria no campo</t>
-  </si>
-  <si>
     <t>MEB correção cliente</t>
   </si>
   <si>
     <t>Daniel Pereira</t>
+  </si>
+  <si>
+    <t>MEB melhoria no campo de filtro no usuario cliente tal</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>124</v>
+        <v>40412</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -533,32 +533,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>167</v>
+        <v>40416</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>167</v>
+        <v>40412</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>